<commit_message>
rundh/rundhshp pyomo 4 only
</commit_message>
<xml_diff>
--- a/mnl.xlsx
+++ b/mnl.xlsx
@@ -953,7 +953,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -985,7 +985,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="5">
-        <v>300</v>
+        <v>1000</v>
       </c>
       <c r="D2" s="10">
         <v>0.01</v>
@@ -999,7 +999,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="5">
-        <v>300</v>
+        <v>1000</v>
       </c>
       <c r="D3" s="10">
         <v>0.01</v>
@@ -1178,7 +1178,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J14" sqref="J14"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>